<commit_message>
Update Design Alternatives Tables.xlsx
</commit_message>
<xml_diff>
--- a/Written Report/Design Alternatives Tables.xlsx
+++ b/Written Report/Design Alternatives Tables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\Capstone\Written Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A92847-B246-4AE7-AD15-2510CAFBB4F4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F60A5E5-B5F8-4478-8BE3-2627903FE7E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,23 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>Drive System</t>
   </si>
   <si>
-    <t>Maneuverability</t>
-  </si>
-  <si>
-    <t>Ease of Implementation</t>
-  </si>
-  <si>
-    <t>Durability</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Total Points</t>
   </si>
   <si>
@@ -68,12 +57,6 @@
     <t>Electronic Control System</t>
   </si>
   <si>
-    <t>Reliability of Control</t>
-  </si>
-  <si>
-    <t>Versatility</t>
-  </si>
-  <si>
     <t>Arduino</t>
   </si>
   <si>
@@ -86,12 +69,6 @@
     <t>Weapon System</t>
   </si>
   <si>
-    <t>Damage</t>
-  </si>
-  <si>
-    <t>Ease of Use</t>
-  </si>
-  <si>
     <t>Hammer</t>
   </si>
   <si>
@@ -110,12 +87,6 @@
     <t>Armor</t>
   </si>
   <si>
-    <t>Strength</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>Aluminum</t>
   </si>
   <si>
@@ -162,6 +133,42 @@
   </si>
   <si>
     <t>Arduino: Radio</t>
+  </si>
+  <si>
+    <t>Maneuverability (Weight 2)</t>
+  </si>
+  <si>
+    <t>Ease of Implementation (Weight 1)</t>
+  </si>
+  <si>
+    <t>Cost (Weight 1)</t>
+  </si>
+  <si>
+    <t>Durability (Weight 2)</t>
+  </si>
+  <si>
+    <t>Ease of Implementation (Weight 2)</t>
+  </si>
+  <si>
+    <t>Reliability of Control (Weight 2)</t>
+  </si>
+  <si>
+    <t>Versatility (Weight 2)</t>
+  </si>
+  <si>
+    <t>Damage (Weight 2)</t>
+  </si>
+  <si>
+    <t>Ease of Use (Weight 2)</t>
+  </si>
+  <si>
+    <t>Strength (Weight 2)</t>
+  </si>
+  <si>
+    <t>Weight (Weight 1)</t>
+  </si>
+  <si>
+    <t>Cost (Weight 2)</t>
   </si>
 </sst>
 </file>
@@ -367,21 +374,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0" tint="-0.249977111117893"/>
       </left>
       <right/>
@@ -654,6 +646,21 @@
         <color theme="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -662,7 +669,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -690,27 +697,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -719,10 +726,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -731,133 +738,139 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1178,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1189,47 +1202,47 @@
     <col min="8" max="13" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="14">
         <v>-1</v>
@@ -1244,103 +1257,107 @@
         <v>2</v>
       </c>
       <c r="F2" s="17">
-        <f>SUM(B2:E2)</f>
-        <v>2</v>
-      </c>
-      <c r="H2" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="57" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="68" t="s">
+        <f>2*B2+C2+2*D2+E2</f>
+        <v>2</v>
+      </c>
+      <c r="H2" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="67"/>
+      <c r="J2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="59"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="54"/>
+        <v>4</v>
+      </c>
+      <c r="H3" s="62"/>
       <c r="I3" s="19">
-        <v>6</v>
+        <f>F4</f>
+        <v>9</v>
       </c>
       <c r="J3" s="8">
-        <v>5</v>
+        <f>F11</f>
+        <v>9</v>
       </c>
       <c r="K3" s="20">
-        <v>5</v>
+        <f>F17</f>
+        <v>9</v>
       </c>
       <c r="L3" s="20">
+        <f>F23</f>
         <v>3</v>
       </c>
       <c r="M3" s="21">
         <f>SUM(I3:L3)</f>
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="23">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24">
+        <v>2</v>
+      </c>
+      <c r="D4" s="24">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="17">
+        <f>2*B4+C4+2*D4+E4</f>
         <v>9</v>
       </c>
-      <c r="B4" s="23">
-        <v>1</v>
-      </c>
-      <c r="C4" s="24">
-        <v>2</v>
-      </c>
-      <c r="D4" s="24">
-        <v>2</v>
-      </c>
-      <c r="E4" s="9">
-        <v>1</v>
-      </c>
-      <c r="F4" s="25">
-        <f>SUM(B4:E4)</f>
-        <v>6</v>
-      </c>
-      <c r="H4" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="61" t="s">
+      <c r="H4" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="61" t="s">
-        <v>29</v>
+      <c r="J4" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="53" t="s">
+        <v>19</v>
       </c>
       <c r="M4" s="25"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" s="19">
         <v>1</v>
@@ -1354,148 +1371,156 @@
       <c r="E5" s="20">
         <v>0</v>
       </c>
-      <c r="F5" s="21">
-        <f>SUM(B5:E5)</f>
-        <v>2</v>
-      </c>
-      <c r="H5" s="56"/>
+      <c r="F5" s="67">
+        <f>2*B5+C5+2*D5+E5</f>
+        <v>3</v>
+      </c>
+      <c r="H5" s="64"/>
       <c r="I5" s="19">
-        <v>0</v>
+        <f>F6</f>
+        <v>1</v>
       </c>
       <c r="J5" s="27">
-        <v>4</v>
+        <f>F13</f>
+        <v>7</v>
       </c>
       <c r="K5" s="20">
-        <v>4</v>
+        <f>F16</f>
+        <v>7</v>
       </c>
       <c r="L5" s="20">
-        <v>1</v>
+        <f>F25</f>
+        <v>2</v>
       </c>
       <c r="M5" s="21">
         <f>SUM(I5:L5)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="48">
+        <v>2</v>
+      </c>
+      <c r="C6" s="39">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="39">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="39">
+        <v>0</v>
+      </c>
+      <c r="F6" s="68">
+        <f>2*B6+C6+2*D6+E6</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="25"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H7" s="66"/>
+      <c r="I7" s="57">
+        <f>F4</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="50">
-        <v>2</v>
-      </c>
-      <c r="C6" s="40">
-        <v>-1</v>
-      </c>
-      <c r="D6" s="40">
-        <v>-1</v>
-      </c>
-      <c r="E6" s="40">
-        <v>0</v>
-      </c>
-      <c r="F6" s="41">
-        <f>SUM(B6:E6)</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="63" t="s">
+      <c r="J7" s="58">
+        <f>F11</f>
+        <v>9</v>
+      </c>
+      <c r="K7" s="58">
+        <f>F18</f>
+        <v>1</v>
+      </c>
+      <c r="L7" s="58">
+        <f>F24</f>
+        <v>3</v>
+      </c>
+      <c r="M7" s="54">
+        <f>SUM(I7:L7)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="64" t="s">
+      <c r="C8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="25"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H7" s="59"/>
-      <c r="I7" s="65">
-        <v>6</v>
-      </c>
-      <c r="J7" s="66">
+      <c r="E8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="41">
+        <v>2</v>
+      </c>
+      <c r="C9" s="42">
+        <v>2</v>
+      </c>
+      <c r="D9" s="43">
+        <v>-2</v>
+      </c>
+      <c r="E9" s="44">
+        <v>1</v>
+      </c>
+      <c r="F9" s="45">
+        <f>2*B9+2*C9+2*D9+E9</f>
         <v>5</v>
-      </c>
-      <c r="K7" s="66">
-        <v>0</v>
-      </c>
-      <c r="L7" s="66">
-        <v>2</v>
-      </c>
-      <c r="M7" s="62">
-        <f>SUM(I7:L7)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="43">
-        <v>2</v>
-      </c>
-      <c r="C9" s="44">
-        <v>2</v>
-      </c>
-      <c r="D9" s="45">
-        <v>-2</v>
-      </c>
-      <c r="E9" s="46">
-        <v>1</v>
-      </c>
-      <c r="F9" s="47">
-        <f>SUM(B9:E9)</f>
-        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B11" s="23">
         <v>1</v>
@@ -1509,14 +1534,14 @@
       <c r="E11" s="9">
         <v>1</v>
       </c>
-      <c r="F11" s="25">
-        <f t="shared" ref="F11:F13" si="0">SUM(B11:E11)</f>
-        <v>5</v>
+      <c r="F11" s="45">
+        <f t="shared" ref="F11:F13" si="0">2*B11+2*C11+2*D11+E11</f>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B12" s="19">
         <v>0</v>
@@ -1530,57 +1555,57 @@
       <c r="E12" s="20">
         <v>1</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="69">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="39">
+      <c r="A13" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="38">
         <v>-1</v>
       </c>
-      <c r="C13" s="49">
-        <v>2</v>
-      </c>
-      <c r="D13" s="49">
-        <v>2</v>
-      </c>
-      <c r="E13" s="40">
-        <v>1</v>
-      </c>
-      <c r="F13" s="41">
+      <c r="C13" s="47">
+        <v>2</v>
+      </c>
+      <c r="D13" s="47">
+        <v>2</v>
+      </c>
+      <c r="E13" s="39">
+        <v>1</v>
+      </c>
+      <c r="F13" s="45">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="36">
+        <v>12</v>
+      </c>
+      <c r="B16" s="35">
         <v>2</v>
       </c>
       <c r="C16" s="15">
@@ -1593,13 +1618,13 @@
         <v>0</v>
       </c>
       <c r="F16" s="17">
-        <f>SUM(B16:E16)</f>
-        <v>4</v>
+        <f>2*B16+C16+2*D16+E16</f>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B17" s="29">
         <v>2</v>
@@ -1613,14 +1638,14 @@
       <c r="E17" s="20">
         <v>0</v>
       </c>
-      <c r="F17" s="21">
-        <f>SUM(B17:E17)</f>
-        <v>5</v>
+      <c r="F17" s="70">
+        <f t="shared" ref="F17:F20" si="1">2*B17+C17+2*D17+E17</f>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B18" s="23">
         <v>0</v>
@@ -1634,14 +1659,14 @@
       <c r="E18" s="9">
         <v>-1</v>
       </c>
-      <c r="F18" s="25">
-        <f>SUM(B18:E18)</f>
-        <v>0</v>
+      <c r="F18" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="37" t="s">
-        <v>24</v>
+      <c r="A19" s="36" t="s">
+        <v>16</v>
       </c>
       <c r="B19" s="19">
         <v>1</v>
@@ -1655,30 +1680,30 @@
       <c r="E19" s="20">
         <v>1</v>
       </c>
-      <c r="F19" s="21">
-        <f>SUM(B19:E19)</f>
+      <c r="F19" s="70">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="39">
-        <v>1</v>
-      </c>
-      <c r="C20" s="40">
+      <c r="A20" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="38">
+        <v>1</v>
+      </c>
+      <c r="C20" s="39">
         <v>0</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="39">
         <v>0</v>
       </c>
-      <c r="E20" s="40">
+      <c r="E20" s="39">
         <v>-1</v>
       </c>
-      <c r="F20" s="41">
-        <f>SUM(B20:E20)</f>
-        <v>0</v>
+      <c r="F20" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1689,31 +1714,31 @@
       <c r="E21" s="4"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="33">
+        <v>18</v>
+      </c>
+      <c r="B23" s="32">
         <v>0</v>
       </c>
       <c r="C23" s="15">
@@ -1726,15 +1751,15 @@
         <v>0</v>
       </c>
       <c r="F23" s="17">
-        <f>SUM(B23:E23)</f>
+        <f>2*B23+C23+D23+2*E23</f>
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="34">
+        <v>23</v>
+      </c>
+      <c r="B24" s="33">
         <v>1</v>
       </c>
       <c r="C24" s="20">
@@ -1746,14 +1771,14 @@
       <c r="E24" s="20">
         <v>0</v>
       </c>
-      <c r="F24" s="21">
-        <f>SUM(B24:E24)</f>
-        <v>2</v>
+      <c r="F24" s="70">
+        <f t="shared" ref="F24:F26" si="2">2*B24+C24+D24+2*E24</f>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B25" s="29">
         <v>2</v>
@@ -1767,14 +1792,14 @@
       <c r="E25" s="9">
         <v>-1</v>
       </c>
-      <c r="F25" s="25">
-        <f>SUM(B25:E25)</f>
-        <v>1</v>
+      <c r="F25" s="17">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="35" t="s">
-        <v>34</v>
+      <c r="A26" s="34" t="s">
+        <v>24</v>
       </c>
       <c r="B26" s="30">
         <v>2</v>
@@ -1788,9 +1813,9 @@
       <c r="E26" s="31">
         <v>0</v>
       </c>
-      <c r="F26" s="32">
-        <f>SUM(B26:E26)</f>
-        <v>0</v>
+      <c r="F26" s="70">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>